<commit_message>
changed to token set ratio
</commit_message>
<xml_diff>
--- a/files/searchNames.xlsx
+++ b/files/searchNames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameschong/Desktop/SanctionListChecker/sanctionlistchecker/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DBB2EBA-E13D-8E4F-866A-C669B4F0B82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179AEB11-E8AB-D140-BD9E-015A83214E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="820" windowWidth="26700" windowHeight="17440" xr2:uid="{9ACEE2C2-942A-684A-B3CA-8969D90CC6A8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -168,13 +168,169 @@
   </si>
   <si>
     <t>Columbia</t>
+  </si>
+  <si>
+    <t>Rishi Gillespie</t>
+  </si>
+  <si>
+    <t>Alessandro Morgan</t>
+  </si>
+  <si>
+    <t>Gauge Camacho</t>
+  </si>
+  <si>
+    <t>Janiya Tanner</t>
+  </si>
+  <si>
+    <t>Samir Hansen</t>
+  </si>
+  <si>
+    <t>Jon Wilkerson</t>
+  </si>
+  <si>
+    <t>Lilyana Silva</t>
+  </si>
+  <si>
+    <t>Quincy Kane</t>
+  </si>
+  <si>
+    <t>Laura Cochran</t>
+  </si>
+  <si>
+    <t>Sergio Becker</t>
+  </si>
+  <si>
+    <t>King Erickson</t>
+  </si>
+  <si>
+    <t>Rihanna Benitez</t>
+  </si>
+  <si>
+    <t>Landin Benjamin</t>
+  </si>
+  <si>
+    <t>Harold Nash</t>
+  </si>
+  <si>
+    <t>Angeline Frye</t>
+  </si>
+  <si>
+    <t>Karlee Carson</t>
+  </si>
+  <si>
+    <t>Leland Trevino</t>
+  </si>
+  <si>
+    <t>Kali Ortiz</t>
+  </si>
+  <si>
+    <t>Asher Sellers</t>
+  </si>
+  <si>
+    <t>Kiley Christian</t>
+  </si>
+  <si>
+    <t>Jamiya Lopez</t>
+  </si>
+  <si>
+    <t>Makenzie Buchanan</t>
+  </si>
+  <si>
+    <t>Xzavier Perry</t>
+  </si>
+  <si>
+    <t>Blaze Fitzpatrick</t>
+  </si>
+  <si>
+    <t>Melvin Schwartz</t>
+  </si>
+  <si>
+    <t>Madeline Blair</t>
+  </si>
+  <si>
+    <t>Sofia Mcguire</t>
+  </si>
+  <si>
+    <t>Dylan Reese</t>
+  </si>
+  <si>
+    <t>Holden Wright</t>
+  </si>
+  <si>
+    <t>Mohamed Thompson</t>
+  </si>
+  <si>
+    <t>Jayvion Velazquez</t>
+  </si>
+  <si>
+    <t>Raegan Mayer</t>
+  </si>
+  <si>
+    <t>Kiana Adkins</t>
+  </si>
+  <si>
+    <t>Tony Marquez</t>
+  </si>
+  <si>
+    <t>Alyson Mccann</t>
+  </si>
+  <si>
+    <t>Gideon Patton</t>
+  </si>
+  <si>
+    <t>Rolando Fitzgerald</t>
+  </si>
+  <si>
+    <t>Aidan Bryan</t>
+  </si>
+  <si>
+    <t>Ray Chaney</t>
+  </si>
+  <si>
+    <t>Maliyah Escobar</t>
+  </si>
+  <si>
+    <t>Micah Oconnell</t>
+  </si>
+  <si>
+    <t>Zayden Fuentes</t>
+  </si>
+  <si>
+    <t>Hadassah Saunders</t>
+  </si>
+  <si>
+    <t>Cassie Moss</t>
+  </si>
+  <si>
+    <t>Annie Barnett</t>
+  </si>
+  <si>
+    <t>Lindsay Dixon</t>
+  </si>
+  <si>
+    <t>Nehemiah Wilson</t>
+  </si>
+  <si>
+    <t>Sean Hester</t>
+  </si>
+  <si>
+    <t>Lola Moses</t>
+  </si>
+  <si>
+    <t>Sergei Ivanov</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Andrei Fursenko</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -193,6 +349,11 @@
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Inherit"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -215,10 +376,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A28B12-B724-D048-B3A7-894DA2A1387D}">
   <dimension ref="A1:M1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:B1001"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="107" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -742,184 +904,439 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" ht="17">
-      <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" ht="17">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" ht="17">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" ht="17">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" ht="17">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" ht="17">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:2" ht="17">
-      <c r="A28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" ht="17">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" ht="17">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:2" ht="17">
-      <c r="A31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" ht="17">
-      <c r="A32" s="2"/>
-    </row>
-    <row r="33" spans="1:1" ht="17">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:1" ht="17">
-      <c r="A34" s="2"/>
-    </row>
-    <row r="35" spans="1:1" ht="17">
-      <c r="A35" s="2"/>
-    </row>
-    <row r="36" spans="1:1" ht="17">
-      <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:1" ht="17">
-      <c r="A37" s="2"/>
-    </row>
-    <row r="38" spans="1:1" ht="17">
-      <c r="A38" s="2"/>
-    </row>
-    <row r="39" spans="1:1" ht="17">
-      <c r="A39" s="2"/>
-    </row>
-    <row r="40" spans="1:1" ht="17">
-      <c r="A40" s="2"/>
-    </row>
-    <row r="41" spans="1:1" ht="17">
-      <c r="A41" s="2"/>
-    </row>
-    <row r="42" spans="1:1" ht="17">
-      <c r="A42" s="2"/>
-    </row>
-    <row r="43" spans="1:1" ht="17">
-      <c r="A43" s="2"/>
-    </row>
-    <row r="44" spans="1:1" ht="17">
-      <c r="A44" s="2"/>
-    </row>
-    <row r="45" spans="1:1" ht="17">
-      <c r="A45" s="2"/>
-    </row>
-    <row r="46" spans="1:1" ht="17">
-      <c r="A46" s="2"/>
-    </row>
-    <row r="47" spans="1:1" ht="17">
-      <c r="A47" s="2"/>
-    </row>
-    <row r="48" spans="1:1" ht="17">
-      <c r="A48" s="2"/>
-    </row>
-    <row r="49" spans="1:1" ht="17">
-      <c r="A49" s="2"/>
-    </row>
-    <row r="50" spans="1:1" ht="17">
-      <c r="A50" s="2"/>
-    </row>
-    <row r="51" spans="1:1" ht="17">
-      <c r="A51" s="2"/>
-    </row>
-    <row r="52" spans="1:1" ht="17">
-      <c r="A52" s="2"/>
-    </row>
-    <row r="53" spans="1:1" ht="17">
-      <c r="A53" s="2"/>
-    </row>
-    <row r="54" spans="1:1" ht="17">
-      <c r="A54" s="2"/>
-    </row>
-    <row r="55" spans="1:1" ht="17">
-      <c r="A55" s="2"/>
-    </row>
-    <row r="56" spans="1:1" ht="17">
-      <c r="A56" s="2"/>
-    </row>
-    <row r="57" spans="1:1" ht="17">
-      <c r="A57" s="2"/>
-    </row>
-    <row r="58" spans="1:1" ht="17">
-      <c r="A58" s="2"/>
-    </row>
-    <row r="59" spans="1:1" ht="17">
-      <c r="A59" s="2"/>
-    </row>
-    <row r="60" spans="1:1" ht="17">
-      <c r="A60" s="2"/>
-    </row>
-    <row r="61" spans="1:1" ht="17">
-      <c r="A61" s="2"/>
-    </row>
-    <row r="62" spans="1:1" ht="17">
-      <c r="A62" s="2"/>
-    </row>
-    <row r="63" spans="1:1" ht="17">
-      <c r="A63" s="2"/>
-    </row>
-    <row r="64" spans="1:1" ht="17">
-      <c r="A64" s="2"/>
-    </row>
-    <row r="65" spans="1:1" ht="17">
-      <c r="A65" s="2"/>
-    </row>
-    <row r="66" spans="1:1" ht="17">
-      <c r="A66" s="2"/>
-    </row>
-    <row r="67" spans="1:1" ht="17">
-      <c r="A67" s="2"/>
-    </row>
-    <row r="68" spans="1:1" ht="17">
-      <c r="A68" s="2"/>
-    </row>
-    <row r="69" spans="1:1" ht="17">
-      <c r="A69" s="2"/>
-    </row>
-    <row r="70" spans="1:1" ht="17">
-      <c r="A70" s="2"/>
-    </row>
-    <row r="71" spans="1:1" ht="17">
-      <c r="A71" s="2"/>
-    </row>
-    <row r="72" spans="1:1" ht="17">
+    <row r="21" spans="1:2" ht="20">
+      <c r="A21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="20">
+      <c r="A22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="20">
+      <c r="A23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="20">
+      <c r="A24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="20">
+      <c r="A25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="20">
+      <c r="A26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="20">
+      <c r="A27" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="20">
+      <c r="A28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="20">
+      <c r="A29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="20">
+      <c r="A30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="20">
+      <c r="A31" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="20">
+      <c r="A32" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="20">
+      <c r="A33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="20">
+      <c r="A34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="20">
+      <c r="A35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="20">
+      <c r="A36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="20">
+      <c r="A37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="20">
+      <c r="A38" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="20">
+      <c r="A39" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="20">
+      <c r="A40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="20">
+      <c r="A41" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="20">
+      <c r="A42" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="20">
+      <c r="A43" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="20">
+      <c r="A44" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="20">
+      <c r="A45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="20">
+      <c r="A46" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="20">
+      <c r="A47" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="20">
+      <c r="A48" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="20">
+      <c r="A49" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="20">
+      <c r="A50" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="20">
+      <c r="A51" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="20">
+      <c r="A52" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="20">
+      <c r="A53" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="20">
+      <c r="A54" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="20">
+      <c r="A55" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="20">
+      <c r="A56" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="20">
+      <c r="A57" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="20">
+      <c r="A58" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="20">
+      <c r="A59" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="20">
+      <c r="A60" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="20">
+      <c r="A61" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="20">
+      <c r="A62" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="20">
+      <c r="A63" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="20">
+      <c r="A64" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B64" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="20">
+      <c r="A65" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B65" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="20">
+      <c r="A66" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="20">
+      <c r="A67" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B67" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="20">
+      <c r="A68" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="20">
+      <c r="A69" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B69" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="20">
+      <c r="A70" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B70" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="17">
+      <c r="A71" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B71" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="17">
       <c r="A72" s="2"/>
     </row>
-    <row r="73" spans="1:1" ht="17">
+    <row r="73" spans="1:2" ht="17">
       <c r="A73" s="2"/>
     </row>
-    <row r="74" spans="1:1" ht="17">
+    <row r="74" spans="1:2" ht="17">
       <c r="A74" s="2"/>
     </row>
-    <row r="75" spans="1:1" ht="17">
+    <row r="75" spans="1:2" ht="17">
       <c r="A75" s="2"/>
     </row>
-    <row r="76" spans="1:1" ht="17">
+    <row r="76" spans="1:2" ht="17">
       <c r="A76" s="2"/>
     </row>
-    <row r="77" spans="1:1" ht="17">
+    <row r="77" spans="1:2" ht="17">
       <c r="A77" s="2"/>
     </row>
-    <row r="78" spans="1:1" ht="17">
+    <row r="78" spans="1:2" ht="17">
       <c r="A78" s="2"/>
     </row>
-    <row r="79" spans="1:1" ht="17">
+    <row r="79" spans="1:2" ht="17">
       <c r="A79" s="2"/>
     </row>
-    <row r="80" spans="1:1" ht="17">
+    <row r="80" spans="1:2" ht="17">
       <c r="A80" s="2"/>
     </row>
     <row r="81" spans="1:1" ht="17">

</xml_diff>